<commit_message>
complete the ood_ness test
</commit_message>
<xml_diff>
--- a/final_ood_casas.xlsx
+++ b/final_ood_casas.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C21"/>
+  <dimension ref="A1:C31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -450,10 +450,10 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>0.5015625</v>
+        <v>0.4965871691703796</v>
       </c>
       <c r="C2" t="n">
-        <v>0.001913663861549358</v>
+        <v>0.006825661659240723</v>
       </c>
     </row>
     <row r="3">
@@ -461,10 +461,10 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>0.6764802631578947</v>
+        <v>0.7680098652839661</v>
       </c>
       <c r="C3" t="n">
-        <v>0.1157950222018389</v>
+        <v>0.1392850526393727</v>
       </c>
     </row>
     <row r="4">
@@ -472,10 +472,10 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>0.7810032894736841</v>
+        <v>0.782154631614685</v>
       </c>
       <c r="C4" t="n">
-        <v>0.03324327075400629</v>
+        <v>0.04232812892036745</v>
       </c>
     </row>
     <row r="5">
@@ -483,10 +483,10 @@
         <v>3</v>
       </c>
       <c r="B5" t="n">
-        <v>0.7717927631578947</v>
+        <v>0.7060444116592407</v>
       </c>
       <c r="C5" t="n">
-        <v>0.1454286532579083</v>
+        <v>0.119835785011813</v>
       </c>
     </row>
     <row r="6">
@@ -494,10 +494,10 @@
         <v>4</v>
       </c>
       <c r="B6" t="n">
-        <v>0.8902549342105264</v>
+        <v>0.8953124761581421</v>
       </c>
       <c r="C6" t="n">
-        <v>0.02864050777323971</v>
+        <v>0.02778017493619667</v>
       </c>
     </row>
     <row r="7">
@@ -505,10 +505,10 @@
         <v>5</v>
       </c>
       <c r="B7" t="n">
-        <v>0.8423519736842107</v>
+        <v>0.9010690808296203</v>
       </c>
       <c r="C7" t="n">
-        <v>0.05860455521331378</v>
+        <v>0.04489960378837834</v>
       </c>
     </row>
     <row r="8">
@@ -516,10 +516,10 @@
         <v>6</v>
       </c>
       <c r="B8" t="n">
-        <v>0.5177631578947368</v>
+        <v>0.5525082230567933</v>
       </c>
       <c r="C8" t="n">
-        <v>0.02399907211243004</v>
+        <v>0.05585504138590723</v>
       </c>
     </row>
     <row r="9">
@@ -527,10 +527,10 @@
         <v>7</v>
       </c>
       <c r="B9" t="n">
-        <v>0.8617187500000002</v>
+        <v>0.9309621691703797</v>
       </c>
       <c r="C9" t="n">
-        <v>0.04108728261753272</v>
+        <v>0.05136255388408779</v>
       </c>
     </row>
     <row r="10">
@@ -538,10 +538,10 @@
         <v>8</v>
       </c>
       <c r="B10" t="n">
-        <v>0.9206825657894736</v>
+        <v>0.9233141303062439</v>
       </c>
       <c r="C10" t="n">
-        <v>0.03516872758721701</v>
+        <v>0.03320143014524354</v>
       </c>
     </row>
     <row r="11">
@@ -549,10 +549,10 @@
         <v>9</v>
       </c>
       <c r="B11" t="n">
-        <v>0.5096628289473684</v>
+        <v>0.5225329041481018</v>
       </c>
       <c r="C11" t="n">
-        <v>0.03546639607580614</v>
+        <v>0.01140590219950456</v>
       </c>
     </row>
     <row r="12">
@@ -560,10 +560,10 @@
         <v>10</v>
       </c>
       <c r="B12" t="n">
-        <v>0.417701344526731</v>
+        <v>0.4038926524777252</v>
       </c>
       <c r="C12" t="n">
-        <v>0.0283990257258962</v>
+        <v>0.0541943277279549</v>
       </c>
     </row>
     <row r="13">
@@ -571,10 +571,10 @@
         <v>11</v>
       </c>
       <c r="B13" t="n">
-        <v>0.6543352442885452</v>
+        <v>0.7513985658799107</v>
       </c>
       <c r="C13" t="n">
-        <v>0.136928483524349</v>
+        <v>0.1653469986355771</v>
       </c>
     </row>
     <row r="14">
@@ -582,10 +582,10 @@
         <v>12</v>
       </c>
       <c r="B14" t="n">
-        <v>0.7784568109523382</v>
+        <v>0.7808253502520608</v>
       </c>
       <c r="C14" t="n">
-        <v>0.03540476223596813</v>
+        <v>0.04249130391582516</v>
       </c>
     </row>
     <row r="15">
@@ -593,10 +593,10 @@
         <v>13</v>
       </c>
       <c r="B15" t="n">
-        <v>0.7542916636835256</v>
+        <v>0.6935019177573688</v>
       </c>
       <c r="C15" t="n">
-        <v>0.1718587398855452</v>
+        <v>0.1295943372390366</v>
       </c>
     </row>
     <row r="16">
@@ -604,10 +604,10 @@
         <v>14</v>
       </c>
       <c r="B16" t="n">
-        <v>0.8900484235690662</v>
+        <v>0.8948479310292814</v>
       </c>
       <c r="C16" t="n">
-        <v>0.02874701006268633</v>
+        <v>0.02811452200975032</v>
       </c>
     </row>
     <row r="17">
@@ -615,10 +615,10 @@
         <v>15</v>
       </c>
       <c r="B17" t="n">
-        <v>0.8382119536665851</v>
+        <v>0.9002750536130222</v>
       </c>
       <c r="C17" t="n">
-        <v>0.06315383678902066</v>
+        <v>0.04519054474493579</v>
       </c>
     </row>
     <row r="18">
@@ -626,10 +626,10 @@
         <v>16</v>
       </c>
       <c r="B18" t="n">
-        <v>0.4416976790493245</v>
+        <v>0.4794554695150628</v>
       </c>
       <c r="C18" t="n">
-        <v>0.0534687805151117</v>
+        <v>0.1035783530436264</v>
       </c>
     </row>
     <row r="19">
@@ -637,10 +637,10 @@
         <v>17</v>
       </c>
       <c r="B19" t="n">
-        <v>0.8598655726359812</v>
+        <v>0.9296867932145789</v>
       </c>
       <c r="C19" t="n">
-        <v>0.04265214256244622</v>
+        <v>0.052589137913941</v>
       </c>
     </row>
     <row r="20">
@@ -648,10 +648,10 @@
         <v>18</v>
       </c>
       <c r="B20" t="n">
-        <v>0.9204532655514768</v>
+        <v>0.9232541603909981</v>
       </c>
       <c r="C20" t="n">
-        <v>0.03524340892053522</v>
+        <v>0.03320371636364689</v>
       </c>
     </row>
     <row r="21">
@@ -659,10 +659,120 @@
         <v>19</v>
       </c>
       <c r="B21" t="n">
-        <v>0.4744863849032885</v>
+        <v>0.4633326887508805</v>
       </c>
       <c r="C21" t="n">
-        <v>0.0497010047123116</v>
+        <v>0.0242152832460079</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="B22" t="n">
+        <v>0.5004718474073753</v>
+      </c>
+      <c r="C22" t="n">
+        <v>0.003803346132688842</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="1" t="n">
+        <v>21</v>
+      </c>
+      <c r="B23" t="n">
+        <v>0.8498151699922092</v>
+      </c>
+      <c r="C23" t="n">
+        <v>0.1500610527910309</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="1" t="n">
+        <v>22</v>
+      </c>
+      <c r="B24" t="n">
+        <v>0.8794450839140409</v>
+      </c>
+      <c r="C24" t="n">
+        <v>0.02949058524935592</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="1" t="n">
+        <v>23</v>
+      </c>
+      <c r="B25" t="n">
+        <v>0.795468317174515</v>
+      </c>
+      <c r="C25" t="n">
+        <v>0.1648746561059093</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="1" t="n">
+        <v>24</v>
+      </c>
+      <c r="B26" t="n">
+        <v>0.9665202048346607</v>
+      </c>
+      <c r="C26" t="n">
+        <v>0.01973715835830648</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="1" t="n">
+        <v>25</v>
+      </c>
+      <c r="B27" t="n">
+        <v>0.9703931137465375</v>
+      </c>
+      <c r="C27" t="n">
+        <v>0.0252654316639312</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="1" t="n">
+        <v>26</v>
+      </c>
+      <c r="B28" t="n">
+        <v>0.6432569847212604</v>
+      </c>
+      <c r="C28" t="n">
+        <v>0.09029948913893696</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="1" t="n">
+        <v>27</v>
+      </c>
+      <c r="B29" t="n">
+        <v>0.9863806050900277</v>
+      </c>
+      <c r="C29" t="n">
+        <v>0.01434377178657925</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="1" t="n">
+        <v>28</v>
+      </c>
+      <c r="B30" t="n">
+        <v>0.9822067472082756</v>
+      </c>
+      <c r="C30" t="n">
+        <v>0.01735241245652931</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="1" t="n">
+        <v>29</v>
+      </c>
+      <c r="B31" t="n">
+        <v>0.497912090438885</v>
+      </c>
+      <c r="C31" t="n">
+        <v>0.04113016954811693</v>
       </c>
     </row>
   </sheetData>

</xml_diff>